<commit_message>
- updates to the .xlsx by Oliver Lenord
git-svn-id: https://openmodelica.org/svn/OpenModelica/trunk/doc@10561 f25d12d1-65f4-0310-ae8a-bbce733d8d8e
</commit_message>
<xml_diff>
--- a/performance/benchmarks/performance.xlsx
+++ b/performance/benchmarks/performance.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -90,8 +90,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +121,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -242,14 +249,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -282,26 +290,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -380,6 +398,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -414,6 +433,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,88 +609,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="2.33203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="1.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="1.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
-      <c r="M1" s="3" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:13">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="M2" s="4" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="O2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="M3" s="5" t="s">
+      <c r="C3" s="21"/>
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="2:13">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1">
-      <c r="F9" s="19" t="s">
+    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="J9" s="19" t="s">
+      <c r="G9" s="23"/>
+      <c r="J9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1">
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>7</v>
       </c>
@@ -691,14 +715,16 @@
         <v>6</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:13">
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>40814</v>
       </c>
@@ -721,15 +747,17 @@
         <v>24091</v>
       </c>
       <c r="J11" s="16">
-        <f t="shared" ref="J11:K14" si="0">F11-F11</f>
+        <f t="shared" ref="J11:J14" si="0">F11-F11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="16">
-        <f t="shared" si="0"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16">
+        <f>G11-G11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E12" s="6" t="s">
         <v>1</v>
       </c>
@@ -746,12 +774,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="6">
-        <f t="shared" si="0"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6">
+        <f>G12-G12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:13">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E13" s="6" t="s">
         <v>2</v>
       </c>
@@ -768,12 +798,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="6">
-        <f t="shared" si="0"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6">
+        <f>G13-G13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:13">
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
@@ -790,13 +822,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="6">
-        <f t="shared" si="0"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6">
+        <f>G14-G14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" ht="15.75" thickBot="1"/>
-    <row r="16" spans="2:13" ht="15.75" thickBot="1">
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
@@ -817,14 +851,16 @@
         <v>6</v>
       </c>
       <c r="I16" s="14"/>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>40867</v>
       </c>
@@ -847,18 +883,26 @@
         <v>28083</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" ref="J17:K20" si="1">F11-F17</f>
+        <f t="shared" ref="J17:J20" si="1">F11-F17</f>
         <v>113</v>
       </c>
-      <c r="K17" s="10">
-        <f t="shared" si="1"/>
+      <c r="K17" s="24">
+        <f>(F17-F11)/F11</f>
+        <v>-0.20545454545454545</v>
+      </c>
+      <c r="L17" s="10">
+        <f>G11-G17</f>
         <v>109</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="24">
+        <f>(G17-G11)/G11</f>
+        <v>-0.1967509025270758</v>
+      </c>
+      <c r="O17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>17</v>
       </c>
@@ -882,12 +926,20 @@
         <f t="shared" si="1"/>
         <v>0.29999999999999982</v>
       </c>
-      <c r="K18" s="8">
-        <f t="shared" si="1"/>
+      <c r="K18" s="24">
+        <f t="shared" ref="K18:M20" si="2">(F18-F12)/F12</f>
+        <v>-4.2253521126760542E-2</v>
+      </c>
+      <c r="L18" s="8">
+        <f>G12-G18</f>
         <v>0.40000000000000036</v>
       </c>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="M18" s="24">
+        <f t="shared" ref="M18:M20" si="3">(G18-G12)/G12</f>
+        <v>-5.3333333333333378E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E19" s="7" t="s">
         <v>2</v>
       </c>
@@ -904,12 +956,20 @@
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="K19" s="8">
-        <f t="shared" si="1"/>
+      <c r="K19" s="24">
+        <f t="shared" si="2"/>
+        <v>-0.20833333333333334</v>
+      </c>
+      <c r="L19" s="8">
+        <f>G13-G19</f>
         <v>2.9000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="2:13">
+      <c r="M19" s="24">
+        <f t="shared" si="3"/>
+        <v>-0.22307692307692312</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E20" s="7" t="s">
         <v>3</v>
       </c>
@@ -926,9 +986,17 @@
         <f t="shared" si="1"/>
         <v>13.8</v>
       </c>
-      <c r="K20" s="8">
-        <f t="shared" si="1"/>
+      <c r="K20" s="24">
+        <f t="shared" si="2"/>
+        <v>-0.57500000000000007</v>
+      </c>
+      <c r="L20" s="8">
+        <f>G14-G20</f>
         <v>13.2</v>
+      </c>
+      <c r="M20" s="24">
+        <f t="shared" si="3"/>
+        <v>-0.54999999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +1004,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -948,24 +1016,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- added comparison to 1.6, 1.7 and one commercial tool.
git-svn-id: https://openmodelica.org/svn/OpenModelica/trunk/doc@10606 f25d12d1-65f4-0310-ae8a-bbce733d8d8e
</commit_message>
<xml_diff>
--- a/performance/benchmarks/performance.xlsx
+++ b/performance/benchmarks/performance.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
   <si>
     <t>HumModOMCTotal</t>
   </si>
@@ -85,13 +85,40 @@
   </si>
   <si>
     <t xml:space="preserve">https://openmodelica.org/svn/OpenModelica/trunk/doc/performance/benchmarks </t>
+  </si>
+  <si>
+    <t>OpenModelica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dymola 7.4 </t>
+  </si>
+  <si>
+    <t>1.6.0</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
+  </si>
+  <si>
+    <t>out of memory</t>
+  </si>
+  <si>
+    <t>max (MB)</t>
+  </si>
+  <si>
+    <t>mem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +156,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +189,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -234,9 +274,48 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -257,7 +336,7 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -272,7 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -283,9 +361,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -297,6 +372,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -306,7 +382,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -321,6 +419,254 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="sv-SE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE" sz="2400"/>
+              <a:t>OpenModelica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sv-SE" sz="2400" baseline="0"/>
+              <a:t> Performance Benchmarks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>checkHumMod</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Data!$B$11,Data!$B$17,Data!$B$23,Data!$B$29,Data!$B$35)</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40814</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40877</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Data!$G$11,Data!$G$17,Data!$G$23,Data!$G$29,Data!$G$35)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2535</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>checkEngineV6</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>(Data!$G$13,Data!$G$19,Data!$G$25,Data!$G$31,Data!$G$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>checkEngineV6_analytic</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>(Data!$G$14,Data!$G$20,Data!$G$26,Data!$G$32,Data!$G$38)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="64745856"/>
+        <c:axId val="64747392"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="64745856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64747392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="64747392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64745856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76670949985418491"/>
+          <c:y val="0.18757882345101781"/>
+          <c:w val="0.20317030046334461"/>
+          <c:h val="9.6976655103252957E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,7 +744,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -433,7 +778,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -609,163 +953,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="1.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O1" s="3" t="s">
+    <row r="1" spans="1:18">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="1:18">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="O2" s="4" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="P2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:18">
+      <c r="B3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="O3" s="5" t="s">
+      <c r="C3" s="20"/>
+      <c r="P3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="1:18">
+      <c r="B4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="P4" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18">
       <c r="B6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="1:18">
+      <c r="B7" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="23" t="s">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="J9" s="23" t="s">
+      <c r="G9" s="22"/>
+      <c r="J9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="20"/>
-    </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="11" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="11" t="s">
+      <c r="K10" s="31"/>
+      <c r="L10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M10" s="31"/>
+      <c r="N10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="B11" s="2">
-        <v>40814</v>
+        <v>40533</v>
       </c>
       <c r="C11" s="1">
-        <v>9944</v>
+        <v>7524</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="16">
-        <f>9*60+10</f>
-        <v>550</v>
-      </c>
-      <c r="G11" s="16">
-        <f>9*60+14</f>
-        <v>554</v>
-      </c>
-      <c r="H11" s="16">
-        <v>24091</v>
-      </c>
-      <c r="J11" s="16">
+      <c r="F11" s="14">
+        <f>49*60+48</f>
+        <v>2988</v>
+      </c>
+      <c r="G11" s="28">
+        <f>65*60+14</f>
+        <v>3914</v>
+      </c>
+      <c r="H11" s="14">
+        <v>24055</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" ref="J11:J14" si="0">F11-F11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16">
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
         <f>G11-G11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M11" s="14"/>
+      <c r="N11" s="14">
+        <f>2.3*1024</f>
+        <v>2355.1999999999998</v>
+      </c>
+      <c r="P11" s="25">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="E12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="6">
-        <v>7.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="G12" s="6">
-        <v>7.5</v>
+        <v>22</v>
       </c>
       <c r="H12" s="6">
         <v>4828</v>
@@ -780,16 +1159,21 @@
         <v>0</v>
       </c>
       <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="N12" s="6"/>
+      <c r="P12" s="25">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="E13" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="6">
-        <v>12</v>
+        <v>34.6</v>
       </c>
       <c r="G13" s="6">
-        <v>13</v>
+        <f>4*60+5</f>
+        <v>245</v>
       </c>
       <c r="H13" s="6">
         <v>12491</v>
@@ -804,16 +1188,21 @@
         <v>0</v>
       </c>
       <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="N13" s="6"/>
+      <c r="P13" s="25">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="6">
-        <v>24</v>
+        <v>27.5</v>
       </c>
       <c r="G14" s="6">
-        <v>24</v>
+        <f>3*60+6</f>
+        <v>186</v>
       </c>
       <c r="H14" s="6">
         <v>9491</v>
@@ -828,183 +1217,742 @@
         <v>0</v>
       </c>
       <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
+      <c r="N14" s="6"/>
+      <c r="P14" s="25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1"/>
+    <row r="16" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="11" t="s">
+      <c r="I16" s="13"/>
+      <c r="J16" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="15"/>
-      <c r="L16" s="11" t="s">
+      <c r="K16" s="31"/>
+      <c r="L16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M16" s="31"/>
+      <c r="N16" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B17" s="2">
+        <v>40653</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8711</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <f>39*60+51</f>
+        <v>2391</v>
+      </c>
+      <c r="G17" s="8">
+        <f>42*60+15</f>
+        <v>2535</v>
+      </c>
+      <c r="H17" s="8">
+        <v>24055</v>
+      </c>
+      <c r="J17" s="9">
+        <f>F11-F17</f>
+        <v>597</v>
+      </c>
+      <c r="K17" s="19">
+        <f>(F17-F11)/F11</f>
+        <v>-0.19979919678714858</v>
+      </c>
+      <c r="L17" s="9">
+        <f>G11-G17</f>
+        <v>1379</v>
+      </c>
+      <c r="M17" s="19">
+        <f>(G17-G11)/G11</f>
+        <v>-0.35232498722534494</v>
+      </c>
+      <c r="N17" s="8">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="B18" s="15"/>
+      <c r="E18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>9.1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>4828</v>
+      </c>
+      <c r="J18" s="9">
+        <f>F12-F18</f>
+        <v>1.0999999999999996</v>
+      </c>
+      <c r="K18" s="19">
+        <f>(F18-F12)/F12</f>
+        <v>-0.10784313725490194</v>
+      </c>
+      <c r="L18" s="9">
+        <f>G12-G18</f>
+        <v>10.5</v>
+      </c>
+      <c r="M18" s="19">
+        <f>(G18-G12)/G12</f>
+        <v>-0.47727272727272729</v>
+      </c>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="E19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7">
+        <v>25.4</v>
+      </c>
+      <c r="G19" s="7">
+        <v>56.4</v>
+      </c>
+      <c r="H19" s="7">
+        <v>12491</v>
+      </c>
+      <c r="J19" s="9">
+        <f>F13-F19</f>
+        <v>9.2000000000000028</v>
+      </c>
+      <c r="K19" s="19">
+        <f>(F19-F13)/F13</f>
+        <v>-0.26589595375722552</v>
+      </c>
+      <c r="L19" s="9">
+        <f>G13-G19</f>
+        <v>188.6</v>
+      </c>
+      <c r="M19" s="19">
+        <f>(G19-G13)/G13</f>
+        <v>-0.76979591836734695</v>
+      </c>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="E20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="7">
+        <v>25.6</v>
+      </c>
+      <c r="G20" s="7">
+        <v>66.7</v>
+      </c>
+      <c r="H20" s="7">
+        <v>9491</v>
+      </c>
+      <c r="J20" s="9">
+        <f>F14-F20</f>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="K20" s="19">
+        <f>(F20-F14)/F14</f>
+        <v>-6.9090909090909036E-2</v>
+      </c>
+      <c r="L20" s="9">
+        <f>G14-G20</f>
+        <v>119.3</v>
+      </c>
+      <c r="M20" s="19">
+        <f>(G20-G14)/G14</f>
+        <v>-0.64139784946236555</v>
+      </c>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A22" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="31"/>
+      <c r="L22" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="31"/>
+      <c r="N22" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2">
+        <v>40814</v>
+      </c>
+      <c r="C23" s="1">
+        <v>9944</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>550</v>
+      </c>
+      <c r="G23" s="8">
+        <v>554</v>
+      </c>
+      <c r="H23" s="8">
+        <v>24091</v>
+      </c>
+      <c r="J23" s="9">
+        <f>F17-F23</f>
+        <v>1841</v>
+      </c>
+      <c r="K23" s="19">
+        <f>(F23-F17)/F17</f>
+        <v>-0.76997072354663321</v>
+      </c>
+      <c r="L23" s="9">
+        <f>G17-G23</f>
+        <v>1981</v>
+      </c>
+      <c r="M23" s="19">
+        <f>(G23-G17)/G17</f>
+        <v>-0.78145956607495071</v>
+      </c>
+      <c r="N23" s="8">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="B24" s="15"/>
+      <c r="E24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="H24" s="7">
+        <v>4828</v>
+      </c>
+      <c r="J24" s="9">
+        <f>F18-F24</f>
+        <v>2</v>
+      </c>
+      <c r="K24" s="19">
+        <f>(F24-F18)/F18</f>
+        <v>-0.21978021978021978</v>
+      </c>
+      <c r="L24" s="9">
+        <f>G18-G24</f>
+        <v>4</v>
+      </c>
+      <c r="M24" s="19">
+        <f>(G24-G18)/G18</f>
+        <v>-0.34782608695652173</v>
+      </c>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="E25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>12</v>
+      </c>
+      <c r="G25" s="7">
+        <v>13</v>
+      </c>
+      <c r="H25" s="7">
+        <v>12491</v>
+      </c>
+      <c r="J25" s="9">
+        <f>F19-F25</f>
+        <v>13.399999999999999</v>
+      </c>
+      <c r="K25" s="19">
+        <f>(F25-F19)/F19</f>
+        <v>-0.52755905511811019</v>
+      </c>
+      <c r="L25" s="9">
+        <f>G19-G25</f>
+        <v>43.4</v>
+      </c>
+      <c r="M25" s="19">
+        <f>(G25-G19)/G19</f>
+        <v>-0.76950354609929073</v>
+      </c>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="E26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
+        <v>24</v>
+      </c>
+      <c r="G26" s="7">
+        <v>24</v>
+      </c>
+      <c r="H26" s="7">
+        <v>9491</v>
+      </c>
+      <c r="J26" s="9">
+        <f>F20-F26</f>
+        <v>1.6000000000000014</v>
+      </c>
+      <c r="K26" s="19">
+        <f>(F26-F20)/F20</f>
+        <v>-6.2500000000000056E-2</v>
+      </c>
+      <c r="L26" s="9">
+        <f>G20-G26</f>
+        <v>42.7</v>
+      </c>
+      <c r="M26" s="19">
+        <f>(G26-G20)/G20</f>
+        <v>-0.64017991004497754</v>
+      </c>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A28" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="31"/>
+      <c r="L28" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="31"/>
+      <c r="N28" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
         <v>40867</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C29" s="1">
         <v>10556</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="9" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F29" s="8">
         <f>7*60+17</f>
         <v>437</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G29" s="8">
         <f>7*60+25</f>
         <v>445</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H29" s="8">
         <v>28083</v>
       </c>
-      <c r="J17" s="10">
-        <f t="shared" ref="J17:J20" si="1">F11-F17</f>
+      <c r="J29" s="9">
+        <f>F23-F29</f>
         <v>113</v>
       </c>
-      <c r="K17" s="24">
-        <f>(F17-F11)/F11</f>
+      <c r="K29" s="19">
+        <f>(F29-F23)/F23</f>
         <v>-0.20545454545454545</v>
       </c>
-      <c r="L17" s="10">
-        <f>G11-G17</f>
+      <c r="L29" s="9">
+        <f>G23-G29</f>
         <v>109</v>
       </c>
-      <c r="M17" s="24">
-        <f>(G17-G11)/G11</f>
+      <c r="M29" s="19">
+        <f>(G29-G23)/G23</f>
         <v>-0.1967509025270758</v>
       </c>
-      <c r="O17" t="s">
+      <c r="N29" s="8">
+        <v>245</v>
+      </c>
+      <c r="P29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
+    <row r="30" spans="1:16">
+      <c r="B30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C18">
-        <f>C17-C11</f>
-        <v>612</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="C30">
+        <f>C29-C11</f>
+        <v>3032</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F30" s="7">
         <v>6.8</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G30" s="7">
         <v>7.1</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H30" s="7">
         <v>4828</v>
       </c>
-      <c r="J18" s="8">
-        <f t="shared" si="1"/>
+      <c r="J30" s="9">
+        <f>F24-F30</f>
         <v>0.29999999999999982</v>
       </c>
-      <c r="K18" s="24">
-        <f t="shared" ref="K18:M20" si="2">(F18-F12)/F12</f>
+      <c r="K30" s="19">
+        <f>(F30-F24)/F24</f>
         <v>-4.2253521126760542E-2</v>
       </c>
-      <c r="L18" s="8">
-        <f>G12-G18</f>
+      <c r="L30" s="9">
+        <f>G24-G30</f>
         <v>0.40000000000000036</v>
       </c>
-      <c r="M18" s="24">
-        <f t="shared" ref="M18:M20" si="3">(G18-G12)/G12</f>
+      <c r="M30" s="19">
+        <f>(G30-G24)/G24</f>
         <v>-5.3333333333333378E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E19" s="7" t="s">
+      <c r="N30" s="7"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="E31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F31" s="7">
         <v>9.5</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G31" s="7">
         <v>10.1</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H31" s="7">
         <v>12491</v>
       </c>
-      <c r="J19" s="8">
-        <f t="shared" si="1"/>
+      <c r="J31" s="9">
+        <f>F25-F31</f>
         <v>2.5</v>
       </c>
-      <c r="K19" s="24">
-        <f t="shared" si="2"/>
+      <c r="K31" s="19">
+        <f>(F31-F25)/F25</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="L19" s="8">
-        <f>G13-G19</f>
+      <c r="L31" s="9">
+        <f>G25-G31</f>
         <v>2.9000000000000004</v>
       </c>
-      <c r="M19" s="24">
-        <f t="shared" si="3"/>
+      <c r="M31" s="19">
+        <f>(G31-G25)/G25</f>
         <v>-0.22307692307692312</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E20" s="7" t="s">
+      <c r="N31" s="7"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="E32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F32" s="7">
         <v>10.199999999999999</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G32" s="7">
         <v>10.8</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H32" s="7">
         <v>9491</v>
       </c>
-      <c r="J20" s="8">
-        <f t="shared" si="1"/>
+      <c r="J32" s="9">
+        <f>F26-F32</f>
         <v>13.8</v>
       </c>
-      <c r="K20" s="24">
-        <f t="shared" si="2"/>
+      <c r="K32" s="19">
+        <f>(F32-F26)/F26</f>
         <v>-0.57500000000000007</v>
       </c>
-      <c r="L20" s="8">
-        <f>G14-G20</f>
+      <c r="L32" s="9">
+        <f>G26-G32</f>
         <v>13.2</v>
       </c>
-      <c r="M20" s="24">
-        <f t="shared" si="3"/>
+      <c r="M32" s="19">
+        <f>(G32-G26)/G26</f>
         <v>-0.54999999999999993</v>
       </c>
+      <c r="N32" s="7"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="34" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A34" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="31"/>
+      <c r="L34" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M34" s="31"/>
+      <c r="N34" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2">
+        <v>40877</v>
+      </c>
+      <c r="C35" s="1">
+        <v>10604</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>46.5</v>
+      </c>
+      <c r="G35" s="8">
+        <v>48.5</v>
+      </c>
+      <c r="H35" s="8">
+        <v>28083</v>
+      </c>
+      <c r="J35" s="9">
+        <f>F29-F35</f>
+        <v>390.5</v>
+      </c>
+      <c r="K35" s="19">
+        <f>(F35-F29)/F29</f>
+        <v>-0.89359267734553771</v>
+      </c>
+      <c r="L35" s="9">
+        <f>G29-G35</f>
+        <v>396.5</v>
+      </c>
+      <c r="M35" s="19">
+        <f>(G35-G29)/G29</f>
+        <v>-0.89101123595505616</v>
+      </c>
+      <c r="N35" s="8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="B36" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <f>C35-C29</f>
+        <v>48</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="G36" s="7">
+        <v>6</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4828</v>
+      </c>
+      <c r="J36" s="9">
+        <f>F30-F36</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="K36" s="19">
+        <f>(F36-F30)/F30</f>
+        <v>-0.17647058823529416</v>
+      </c>
+      <c r="L36" s="9">
+        <f>G30-G36</f>
+        <v>1.0999999999999996</v>
+      </c>
+      <c r="M36" s="19">
+        <f>(G36-G30)/G30</f>
+        <v>-0.15492957746478869</v>
+      </c>
+      <c r="N36" s="7"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="E37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G37" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H37" s="7">
+        <v>12491</v>
+      </c>
+      <c r="J37" s="9">
+        <f>F31-F37</f>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="K37" s="19">
+        <f>(F37-F31)/F31</f>
+        <v>-7.3684210526315713E-2</v>
+      </c>
+      <c r="L37" s="9">
+        <f>G31-G37</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="M37" s="19">
+        <f>(G37-G31)/G31</f>
+        <v>-3.9603960396039639E-2</v>
+      </c>
+      <c r="N37" s="7"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="E38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="G38" s="7">
+        <v>10.3</v>
+      </c>
+      <c r="H38" s="7">
+        <v>9491</v>
+      </c>
+      <c r="J38" s="9">
+        <f>F32-F38</f>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="K38" s="19">
+        <f>(F38-F32)/F32</f>
+        <v>-5.8823529411764677E-2</v>
+      </c>
+      <c r="L38" s="9">
+        <f>G32-G38</f>
+        <v>0.5</v>
+      </c>
+      <c r="M38" s="19">
+        <f>(G38-G32)/G32</f>
+        <v>-4.6296296296296294E-2</v>
+      </c>
+      <c r="N38" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -1016,24 +1964,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- update performance figures.
git-svn-id: https://openmodelica.org/svn/OpenModelica/trunk/doc@12694 f25d12d1-65f4-0310-ae8a-bbce733d8d8e
</commit_message>
<xml_diff>
--- a/performance/benchmarks/performance.xlsx
+++ b/performance/benchmarks/performance.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
   <si>
     <t>HumModOMCTotal</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>mem</t>
+  </si>
+  <si>
+    <t>1.9.0</t>
+  </si>
+  <si>
+    <t>1.8.1</t>
   </si>
 </sst>
 </file>
@@ -185,13 +191,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +342,7 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -344,9 +350,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -386,14 +389,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -403,6 +400,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,7 +433,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -569,11 +579,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104532224"/>
-        <c:axId val="104550400"/>
+        <c:axId val="204974720"/>
+        <c:axId val="204988800"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104532224"/>
+        <c:axId val="204974720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,17 +597,17 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="sv-SE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104550400"/>
+        <c:crossAx val="204988800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104550400"/>
+        <c:axId val="204988800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -606,7 +616,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104532224"/>
+        <c:crossAx val="204974720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -617,10 +627,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77712616652085154"/>
-          <c:y val="0.12363900210640101"/>
+          <c:x val="0.77712616652085165"/>
+          <c:y val="0.12363900210640102"/>
           <c:w val="0.20317030046334461"/>
-          <c:h val="9.6976655103252984E-2"/>
+          <c:h val="9.6976655103253026E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -629,7 +639,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -955,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -986,35 +996,35 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="P2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="P3" s="5" t="s">
+      <c r="C3" s="26"/>
+      <c r="P3" s="35" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="P4" s="26" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="P4" s="25" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1029,7 +1039,7 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1037,60 +1047,60 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="J9" s="31" t="s">
+      <c r="G9" s="28"/>
+      <c r="J9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="18"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="23" t="s">
         <v>24</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="27" t="s">
+      <c r="I10" s="12"/>
+      <c r="J10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27" t="s">
+      <c r="K10" s="30"/>
+      <c r="L10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="28"/>
-      <c r="N10" s="20" t="s">
+      <c r="M10" s="30"/>
+      <c r="N10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="P10" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1105,158 +1115,158 @@
         <v>7524</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <f>49*60+48</f>
         <v>2988</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="24">
         <f>65*60+14</f>
         <v>3914</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>24055</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <f t="shared" ref="J11:J14" si="0">F11-F11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13">
         <f>G11-G11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14">
+      <c r="M11" s="13"/>
+      <c r="N11" s="13">
         <f>2.3*1024</f>
         <v>2355.1999999999998</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="21">
         <v>13.95</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>10.199999999999999</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>22</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>4828</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5">
         <f>G12-G12</f>
         <v>0</v>
       </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="P12" s="22">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="P12" s="21">
         <v>4.68</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>34.6</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f>4*60+5</f>
         <v>245</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>12491</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5">
         <f>G13-G13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="P13" s="22">
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="P13" s="21">
         <v>2.6</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>27.5</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f>3*60+6</f>
         <v>186</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>9491</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
         <f>G14-G14</f>
         <v>0</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="P14" s="22">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="P14" s="21">
         <v>2.4</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="16" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12" t="s">
+      <c r="D16" s="10"/>
+      <c r="E16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="27" t="s">
+      <c r="I16" s="12"/>
+      <c r="J16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27" t="s">
+      <c r="K16" s="30"/>
+      <c r="L16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="28"/>
-      <c r="N16" s="20" t="s">
+      <c r="M16" s="30"/>
+      <c r="N16" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1271,168 +1281,168 @@
         <v>8711</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <f>39*60+51</f>
         <v>2391</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <f>42*60+15</f>
         <v>2535</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>24055</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <f>F11-F17</f>
         <v>597</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <f>(F17-F11)/F11</f>
         <v>-0.19979919678714858</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="8">
         <f>G11-G17</f>
         <v>1379</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="18">
         <f>(G17-G11)/G11</f>
         <v>-0.35232498722534494</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="7">
         <v>675</v>
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="B18" s="15"/>
-      <c r="E18" s="7" t="s">
+      <c r="B18" s="14"/>
+      <c r="E18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>9.1</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>11.5</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>4828</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <f>F12-F18</f>
         <v>1.0999999999999996</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="18">
         <f>(F18-F12)/F12</f>
         <v>-0.10784313725490194</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="8">
         <f>G12-G18</f>
         <v>10.5</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="18">
         <f>(G18-G12)/G12</f>
         <v>-0.47727272727272729</v>
       </c>
-      <c r="N18" s="7"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>25.4</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>56.4</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>12491</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <f>F13-F19</f>
         <v>9.2000000000000028</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="18">
         <f>(F19-F13)/F13</f>
         <v>-0.26589595375722552</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <f>G13-G19</f>
         <v>188.6</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="18">
         <f>(G19-G13)/G13</f>
         <v>-0.76979591836734695</v>
       </c>
-      <c r="N19" s="7"/>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>25.6</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>66.7</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>9491</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <f>F14-F20</f>
         <v>1.8999999999999986</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="18">
         <f>(F20-F14)/F14</f>
         <v>-6.9090909090909036E-2</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <f>G14-G20</f>
         <v>119.3</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="18">
         <f>(G20-G14)/G14</f>
         <v>-0.64139784946236555</v>
       </c>
-      <c r="N20" s="7"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="22" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="10"/>
+      <c r="E22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="27" t="s">
+      <c r="I22" s="12"/>
+      <c r="J22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27" t="s">
+      <c r="K22" s="30"/>
+      <c r="L22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="28"/>
-      <c r="N22" s="20" t="s">
+      <c r="M22" s="30"/>
+      <c r="N22" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1447,166 +1457,166 @@
         <v>9944</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>550</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>554</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>24091</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="8">
         <f>F17-F23</f>
         <v>1841</v>
       </c>
-      <c r="K23" s="19">
+      <c r="K23" s="18">
         <f>(F23-F17)/F17</f>
         <v>-0.76997072354663321</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="8">
         <f>G17-G23</f>
         <v>1981</v>
       </c>
-      <c r="M23" s="19">
+      <c r="M23" s="18">
         <f>(G23-G17)/G17</f>
         <v>-0.78145956607495071</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="7">
         <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="B24" s="15"/>
-      <c r="E24" s="7" t="s">
+      <c r="B24" s="14"/>
+      <c r="E24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>7.1</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>7.5</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>4828</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <f>F18-F24</f>
         <v>2</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="18">
         <f>(F24-F18)/F18</f>
         <v>-0.21978021978021978</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="8">
         <f>G18-G24</f>
         <v>4</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="18">
         <f>(G24-G18)/G18</f>
         <v>-0.34782608695652173</v>
       </c>
-      <c r="N24" s="7"/>
+      <c r="N24" s="6"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>12</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>13</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="6">
         <v>12491</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <f>F19-F25</f>
         <v>13.399999999999999</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="18">
         <f>(F25-F19)/F19</f>
         <v>-0.52755905511811019</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="8">
         <f>G19-G25</f>
         <v>43.4</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="18">
         <f>(G25-G19)/G19</f>
         <v>-0.76950354609929073</v>
       </c>
-      <c r="N25" s="7"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>24</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>24</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="6">
         <v>9491</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <f>F20-F26</f>
         <v>1.6000000000000014</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="18">
         <f>(F26-F20)/F20</f>
         <v>-6.2500000000000056E-2</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="8">
         <f>G20-G26</f>
         <v>42.7</v>
       </c>
-      <c r="M26" s="19">
+      <c r="M26" s="18">
         <f>(G26-G20)/G20</f>
         <v>-0.64017991004497754</v>
       </c>
-      <c r="N26" s="7"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="28" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="27" t="s">
+      <c r="I28" s="12"/>
+      <c r="J28" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="28"/>
-      <c r="L28" s="27" t="s">
+      <c r="K28" s="30"/>
+      <c r="L28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="20" t="s">
+      <c r="M28" s="30"/>
+      <c r="N28" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1621,37 +1631,37 @@
         <v>10556</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <f>7*60+17</f>
         <v>437</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <f>7*60+25</f>
         <v>445</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="7">
         <v>28083</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <f>F23-F29</f>
         <v>113</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="18">
         <f>(F29-F23)/F23</f>
         <v>-0.20545454545454545</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="8">
         <f>G23-G29</f>
         <v>109</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="18">
         <f>(G29-G23)/G23</f>
         <v>-0.1967509025270758</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="7">
         <v>245</v>
       </c>
       <c r="P29" t="s">
@@ -1659,139 +1669,139 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C30">
         <f>C29-C11</f>
         <v>3032</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>6.8</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>7.1</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="6">
         <v>4828</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <f>F24-F30</f>
         <v>0.29999999999999982</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="18">
         <f>(F30-F24)/F24</f>
         <v>-4.2253521126760542E-2</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="8">
         <f>G24-G30</f>
         <v>0.40000000000000036</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="18">
         <f>(G30-G24)/G24</f>
         <v>-5.3333333333333378E-2</v>
       </c>
-      <c r="N30" s="7"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>9.5</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>10.1</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="6">
         <v>12491</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <f>F25-F31</f>
         <v>2.5</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="18">
         <f>(F31-F25)/F25</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="8">
         <f>G25-G31</f>
         <v>2.9000000000000004</v>
       </c>
-      <c r="M31" s="19">
+      <c r="M31" s="18">
         <f>(G31-G25)/G25</f>
         <v>-0.22307692307692312</v>
       </c>
-      <c r="N31" s="7"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>10.8</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="6">
         <v>9491</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="8">
         <f>F26-F32</f>
         <v>13.8</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="18">
         <f>(F32-F26)/F26</f>
         <v>-0.57500000000000007</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="8">
         <f>G26-G32</f>
         <v>13.2</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="18">
         <f>(G32-G26)/G26</f>
         <v>-0.54999999999999993</v>
       </c>
-      <c r="N32" s="7"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="34" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12" t="s">
+      <c r="D34" s="10"/>
+      <c r="E34" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="27" t="s">
+      <c r="I34" s="12"/>
+      <c r="J34" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="28"/>
-      <c r="L34" s="27" t="s">
+      <c r="K34" s="30"/>
+      <c r="L34" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M34" s="28"/>
-      <c r="N34" s="20" t="s">
+      <c r="M34" s="30"/>
+      <c r="N34" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1806,146 +1816,500 @@
         <v>10604</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>46.5</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <v>48.5</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="7">
         <v>28083</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="8">
         <f>F29-F35</f>
         <v>390.5</v>
       </c>
-      <c r="K35" s="19">
+      <c r="K35" s="18">
         <f>(F35-F29)/F29</f>
         <v>-0.89359267734553771</v>
       </c>
-      <c r="L35" s="9">
+      <c r="L35" s="8">
         <f>G29-G35</f>
         <v>396.5</v>
       </c>
-      <c r="M35" s="19">
+      <c r="M35" s="18">
         <f>(G35-G29)/G29</f>
         <v>-0.89101123595505616</v>
       </c>
-      <c r="N35" s="8">
+      <c r="N35" s="7">
         <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:14">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C36">
         <f>C35-C29</f>
         <v>48</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>5.6</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="6">
         <v>6</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="6">
         <v>4828</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J36" s="8">
         <f>F30-F36</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K36" s="19">
+      <c r="K36" s="18">
         <f>(F36-F30)/F30</f>
         <v>-0.17647058823529416</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="8">
         <f>G30-G36</f>
         <v>1.0999999999999996</v>
       </c>
-      <c r="M36" s="19">
+      <c r="M36" s="18">
         <f>(G36-G30)/G30</f>
         <v>-0.15492957746478869</v>
       </c>
-      <c r="N36" s="7"/>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="6">
         <v>12491</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="8">
         <f>F31-F37</f>
         <v>0.69999999999999929</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="18">
         <f>(F37-F31)/F31</f>
         <v>-7.3684210526315713E-2</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="8">
         <f>G31-G37</f>
         <v>0.40000000000000036</v>
       </c>
-      <c r="M37" s="19">
+      <c r="M37" s="18">
         <f>(G37-G31)/G31</f>
         <v>-3.9603960396039639E-2</v>
       </c>
-      <c r="N37" s="7"/>
+      <c r="N37" s="6"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>9.6</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <v>10.3</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="6">
         <v>9491</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="8">
         <f>F32-F38</f>
         <v>0.59999999999999964</v>
       </c>
-      <c r="K38" s="19">
+      <c r="K38" s="18">
         <f>(F38-F32)/F32</f>
         <v>-5.8823529411764677E-2</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38" s="8">
         <f>G32-G38</f>
         <v>0.5</v>
       </c>
-      <c r="M38" s="19">
+      <c r="M38" s="18">
         <f>(G38-G32)/G32</f>
         <v>-4.6296296296296294E-2</v>
       </c>
-      <c r="N38" s="7"/>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="40" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A40" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="12"/>
+      <c r="J40" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="30"/>
+      <c r="L40" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="M40" s="30"/>
+      <c r="N40" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="2">
+        <v>41087</v>
+      </c>
+      <c r="C41" s="1">
+        <v>12214</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>49</v>
+      </c>
+      <c r="G41" s="7">
+        <v>51.4</v>
+      </c>
+      <c r="H41" s="7">
+        <v>28083</v>
+      </c>
+      <c r="J41" s="31">
+        <f>F35-F41</f>
+        <v>-2.5</v>
+      </c>
+      <c r="K41" s="32">
+        <f>(F41-F35)/F35</f>
+        <v>5.3763440860215055E-2</v>
+      </c>
+      <c r="L41" s="31">
+        <f>G35-G41</f>
+        <v>-2.8999999999999986</v>
+      </c>
+      <c r="M41" s="32">
+        <f>(G41-G35)/G35</f>
+        <v>5.9793814432989659E-2</v>
+      </c>
+      <c r="N41" s="33"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <f>C41-C35</f>
+        <v>1610</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>7.95</v>
+      </c>
+      <c r="G42" s="6">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="H42" s="6">
+        <v>4828</v>
+      </c>
+      <c r="J42" s="31">
+        <f>F36-F42</f>
+        <v>-2.3500000000000005</v>
+      </c>
+      <c r="K42" s="32">
+        <f>(F42-F36)/F36</f>
+        <v>0.41964285714285726</v>
+      </c>
+      <c r="L42" s="31">
+        <f>G36-G42</f>
+        <v>-2.7200000000000006</v>
+      </c>
+      <c r="M42" s="32">
+        <f>(G42-G36)/G36</f>
+        <v>0.45333333333333342</v>
+      </c>
+      <c r="N42" s="34"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="E43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="6">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="G43" s="6">
+        <v>11</v>
+      </c>
+      <c r="H43" s="6">
+        <v>12491</v>
+      </c>
+      <c r="J43" s="31">
+        <f>F37-F43</f>
+        <v>-1.42</v>
+      </c>
+      <c r="K43" s="32">
+        <f>(F43-F37)/F37</f>
+        <v>0.16136363636363635</v>
+      </c>
+      <c r="L43" s="31">
+        <f>G37-G43</f>
+        <v>-1.3000000000000007</v>
+      </c>
+      <c r="M43" s="32">
+        <f>(G43-G37)/G37</f>
+        <v>0.13402061855670111</v>
+      </c>
+      <c r="N43" s="34"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="E44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="6">
+        <v>10.94</v>
+      </c>
+      <c r="G44" s="6">
+        <v>11.81</v>
+      </c>
+      <c r="H44" s="6">
+        <v>9491</v>
+      </c>
+      <c r="J44" s="31">
+        <f>F38-F44</f>
+        <v>-1.3399999999999999</v>
+      </c>
+      <c r="K44" s="32">
+        <f>(F44-F38)/F38</f>
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="L44" s="31">
+        <f>G38-G44</f>
+        <v>-1.5099999999999998</v>
+      </c>
+      <c r="M44" s="32">
+        <f>(G44-G38)/G38</f>
+        <v>0.14660194174757279</v>
+      </c>
+      <c r="N44" s="34"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A46" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="12"/>
+      <c r="J46" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K46" s="30"/>
+      <c r="L46" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" s="30"/>
+      <c r="N46" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="2">
+        <v>41149</v>
+      </c>
+      <c r="C47" s="1">
+        <v>12693</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="7">
+        <v>50.87</v>
+      </c>
+      <c r="G47" s="7">
+        <v>49.06</v>
+      </c>
+      <c r="H47" s="7">
+        <v>28083</v>
+      </c>
+      <c r="J47" s="31">
+        <f>F41-F47</f>
+        <v>-1.8699999999999974</v>
+      </c>
+      <c r="K47" s="32">
+        <f>(F47-F41)/F41</f>
+        <v>3.81632653061224E-2</v>
+      </c>
+      <c r="L47" s="8">
+        <f>G41-G47</f>
+        <v>2.3399999999999963</v>
+      </c>
+      <c r="M47" s="18">
+        <f>(G47-G41)/G41</f>
+        <v>-4.5525291828793703E-2</v>
+      </c>
+      <c r="N47" s="7"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="B48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48">
+        <f>C47-C41</f>
+        <v>479</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6">
+        <v>7.78</v>
+      </c>
+      <c r="G48" s="6">
+        <v>7.49</v>
+      </c>
+      <c r="H48" s="6">
+        <v>4828</v>
+      </c>
+      <c r="J48" s="8">
+        <f>F42-F48</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="K48" s="18">
+        <f>(F48-F42)/F42</f>
+        <v>-2.138364779874213E-2</v>
+      </c>
+      <c r="L48" s="8">
+        <f>G42-G48</f>
+        <v>1.2300000000000004</v>
+      </c>
+      <c r="M48" s="18">
+        <f>(G48-G42)/G42</f>
+        <v>-0.14105504587155968</v>
+      </c>
+      <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="5:14">
+      <c r="E49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="6">
+        <v>10.6</v>
+      </c>
+      <c r="G49" s="6">
+        <v>9.9</v>
+      </c>
+      <c r="H49" s="6">
+        <v>12491</v>
+      </c>
+      <c r="J49" s="31">
+        <f>F43-F49</f>
+        <v>-0.37999999999999901</v>
+      </c>
+      <c r="K49" s="32">
+        <f>(F49-F43)/F43</f>
+        <v>3.7181996086105576E-2</v>
+      </c>
+      <c r="L49" s="8">
+        <f>G43-G49</f>
+        <v>1.0999999999999996</v>
+      </c>
+      <c r="M49" s="18">
+        <f>(G49-G43)/G43</f>
+        <v>-9.9999999999999964E-2</v>
+      </c>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="5:14">
+      <c r="E50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="6">
+        <v>11.35</v>
+      </c>
+      <c r="G50" s="6">
+        <v>11.05</v>
+      </c>
+      <c r="H50" s="6">
+        <v>9491</v>
+      </c>
+      <c r="J50" s="31">
+        <f>F44-F50</f>
+        <v>-0.41000000000000014</v>
+      </c>
+      <c r="K50" s="32">
+        <f>(F50-F44)/F44</f>
+        <v>3.7477148080438769E-2</v>
+      </c>
+      <c r="L50" s="8">
+        <f>G44-G50</f>
+        <v>0.75999999999999979</v>
+      </c>
+      <c r="M50" s="18">
+        <f>(G50-G44)/G44</f>
+        <v>-6.4352243861134611E-2</v>
+      </c>
+      <c r="N50" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
+  <mergeCells count="18">
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="J16:K16"/>
@@ -1954,6 +2318,12 @@
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="L28:M28"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -1968,7 +2338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>

</xml_diff>